<commit_message>
feat: add CyberRiskScore and DeviceTrustScore to ML_Features, rm admin/data_generator from repo
</commit_message>
<xml_diff>
--- a/bank/flux_financial_database.xlsx
+++ b/bank/flux_financial_database.xlsx
@@ -668,17 +668,17 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
+          <t>CyberRiskScore</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>DeviceTrustScore</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
           <t>RiskLabel</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>CyberRiskScore</t>
-        </is>
-      </c>
-      <c r="M1" t="inlineStr">
-        <is>
-          <t>DeviceTrustScore</t>
         </is>
       </c>
     </row>

</xml_diff>